<commit_message>
nb: adding all updated elo score nb to jn folder
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/ELO_score/data/Urine_Marking_Assay_Data.xlsx
+++ b/jupyter_notebooks/ELO_score/data/Urine_Marking_Assay_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida.sharepoint.com/teams/Padilla-CoreanoLab/Shared Documents/General/Data/Pilot - C57 vs CD1 Dominance Behavior Comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="536" documentId="8_{FDCD49E8-D898-4C16-88FE-ACF6D76972A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D53659AE-48C1-4835-8798-503CE48FD785}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="6_{3CCD3330-EE46-D54B-987A-6296EAF92943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC15BDFF-FF5D-4639-A974-96D4FF38F7E5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" firstSheet="2" activeTab="5" xr2:uid="{07FA63AF-F3ED-490A-A216-EB94940CA1E8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" firstSheet="5" activeTab="3" xr2:uid="{07FA63AF-F3ED-490A-A216-EB94940CA1E8}"/>
   </bookViews>
   <sheets>
     <sheet name="CAGE1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="54">
   <si>
     <t>urine marking assay</t>
   </si>
@@ -96,13 +96,19 @@
     <t>4vs1</t>
   </si>
   <si>
+    <t xml:space="preserve">Subject </t>
+  </si>
+  <si>
+    <t>WINS</t>
+  </si>
+  <si>
     <t>2vs4</t>
   </si>
   <si>
-    <t xml:space="preserve">Subject </t>
-  </si>
-  <si>
-    <t>WINS</t>
+    <t>1v2</t>
+  </si>
+  <si>
+    <t>3v4</t>
   </si>
   <si>
     <t>WINNER (Who has the most spots)</t>
@@ -147,6 +153,9 @@
     <t>repeting day 3 medpc</t>
   </si>
   <si>
+    <t>Subjects</t>
+  </si>
+  <si>
     <t>4v1</t>
   </si>
   <si>
@@ -157,9 +166,6 @@
   </si>
   <si>
     <t xml:space="preserve">repeting day 3 medpc, </t>
-  </si>
-  <si>
-    <t>Subjects</t>
   </si>
   <si>
     <t>Notes (holes..etc)</t>
@@ -202,10 +208,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -231,9 +244,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,15 +563,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214F54E8-2922-4EF0-813F-02E01555FEBB}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="G9" sqref="G9:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.42578125" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" customWidth="1"/>
     <col min="5" max="6" width="12.28515625" customWidth="1"/>
@@ -724,6 +739,12 @@
       <c r="F9">
         <v>1</v>
       </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1">
@@ -744,13 +765,19 @@
       <c r="F10">
         <v>3</v>
       </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>44776</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>14</v>
@@ -763,6 +790,12 @@
       </c>
       <c r="F11">
         <v>2</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -784,11 +817,11 @@
       <c r="F12">
         <v>3</v>
       </c>
-      <c r="G12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" t="s">
-        <v>20</v>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -811,34 +844,50 @@
         <v>4</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="H14">
-        <v>4</v>
+      <c r="A14" s="1">
+        <v>44778</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="G15">
-        <v>3</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="G16">
-        <v>4</v>
-      </c>
-      <c r="H16">
-        <v>2</v>
+      <c r="A15" s="1">
+        <v>44778</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -848,10 +897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C0ED53-4AA2-46CE-B2C4-A119DA7664CC}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H10" sqref="H10:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -876,10 +925,10 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1019,10 +1068,10 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1044,13 +1093,19 @@
       <c r="F10">
         <v>3</v>
       </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>44776</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>9</v>
@@ -1063,6 +1118,12 @@
       </c>
       <c r="F11">
         <v>4</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1084,11 +1145,11 @@
       <c r="F12">
         <v>2</v>
       </c>
-      <c r="H12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" t="s">
-        <v>20</v>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1111,34 +1172,56 @@
         <v>4</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I13">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:9">
+      <c r="A14" s="1">
+        <v>44778</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
       <c r="H14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="H16">
-        <v>4</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
+      <c r="A15" s="1">
+        <v>44778</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>132</v>
+      </c>
+      <c r="D15">
+        <v>28</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1148,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE360E41-2601-4749-8928-EBA54CE18A83}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G10" sqref="G10:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1176,10 +1259,10 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1344,6 +1427,12 @@
       <c r="F10">
         <v>3</v>
       </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1">
@@ -1364,6 +1453,12 @@
       <c r="F11">
         <v>2</v>
       </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1">
@@ -1384,11 +1479,11 @@
       <c r="F12">
         <v>2</v>
       </c>
-      <c r="G12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" t="s">
-        <v>26</v>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1411,34 +1506,56 @@
         <v>4</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:8">
+      <c r="A14" s="2">
+        <v>44778</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
       <c r="G14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="G15">
-        <v>3</v>
-      </c>
-      <c r="H15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="G16">
-        <v>4</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
+      <c r="A15" s="2">
+        <v>44778</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>44</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1448,10 +1565,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69429A73-70A4-417B-9EE0-E79ECB0E6855}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1476,10 +1593,10 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1525,7 +1642,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1548,7 +1665,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1599,13 +1716,13 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1616,13 +1733,13 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1630,7 +1747,7 @@
         <v>44756</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10">
         <v>76</v>
@@ -1645,7 +1762,13 @@
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1653,16 +1776,22 @@
         <v>44756</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1670,7 +1799,7 @@
         <v>44757</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C12">
         <v>8</v>
@@ -1685,7 +1814,13 @@
         <v>4</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1707,13 +1842,19 @@
       <c r="F13">
         <v>3</v>
       </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>44776</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <v>194</v>
@@ -1726,6 +1867,12 @@
       </c>
       <c r="F14">
         <v>4</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1735,6 +1882,15 @@
       <c r="B15" t="s">
         <v>16</v>
       </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1">
@@ -1743,43 +1899,54 @@
       <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="I16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="9:10">
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="9:10">
-      <c r="I18">
-        <v>2</v>
-      </c>
-      <c r="J18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="9:10">
-      <c r="I19">
-        <v>3</v>
-      </c>
-      <c r="J19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="9:10">
-      <c r="I20">
-        <v>4</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>44778</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>247</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>44778</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <v>13</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1789,10 +1956,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E739AF-AEC0-4DAC-861E-EE7592D21DB6}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C411" sqref="C411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1817,10 +1984,10 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1866,7 +2033,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1889,7 +2056,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1900,19 +2067,19 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1923,13 +2090,13 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1958,7 +2125,7 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J8">
         <v>2</v>
@@ -1987,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J9">
         <v>3</v>
@@ -2001,7 +2168,7 @@
         <v>44756</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -2016,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J10">
         <v>4</v>
@@ -2030,7 +2197,7 @@
         <v>44756</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2045,7 +2212,7 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2073,7 +2240,7 @@
         <v>44776</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -2126,6 +2293,46 @@
       </c>
       <c r="F15">
         <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="2">
+        <v>44778</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>247</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2">
+        <v>44778</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>33</v>
+      </c>
+      <c r="D17">
+        <v>13</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2135,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001AAB5C-14E1-449B-8322-A401ED4EFE37}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2161,10 +2368,10 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2244,13 +2451,13 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -2273,10 +2480,10 @@
         <v>2</v>
       </c>
       <c r="K7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2325,7 +2532,7 @@
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K9">
         <v>2</v>
@@ -2365,7 +2572,7 @@
         <v>44776</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>8</v>
@@ -2424,6 +2631,46 @@
       </c>
       <c r="F13">
         <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="2">
+        <v>44778</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>81</v>
+      </c>
+      <c r="D14">
+        <v>37</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="2">
+        <v>44778</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>53</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2432,17 +2679,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="05f64c5e-7ec2-4cf0-a148-a77e53878df3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002C00C86E44419345A6E3C05C9040286D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="65c1c2793603bcc5a4934c5d6e8e8f06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="05f64c5e-7ec2-4cf0-a148-a77e53878df3" xmlns:ns3="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6cc1102e38a8cc84e5ccb56329e356c" ns2:_="" ns3:_="">
     <xsd:import namespace="05f64c5e-7ec2-4cf0-a148-a77e53878df3"/>
@@ -2679,7 +2915,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2688,14 +2924,25 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="05f64c5e-7ec2-4cf0-a148-a77e53878df3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39166E05-9E46-4D8A-A3C4-43A0AE3AE29E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEEA5219-C4E2-42CD-B312-67502A76525D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEEA5219-C4E2-42CD-B312-67502A76525D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47F57269-D722-4DA7-BC1C-3CBD76C00C24}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47F57269-D722-4DA7-BC1C-3CBD76C00C24}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39166E05-9E46-4D8A-A3C4-43A0AE3AE29E}"/>
 </file>
</xml_diff>